<commit_message>
fixed excel filter to correctly output every trip in database tables
</commit_message>
<xml_diff>
--- a/database/Example_Data/TripsAndLeaderStatusInfo.xlsx
+++ b/database/Example_Data/TripsAndLeaderStatusInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lduli\TripPrefVisualizer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lduli\TripPrefVisualizer\database\Example_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D14B149-6742-4859-83D5-E598D3591C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2638FF-8396-44EC-9588-851A3DF13B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" activeTab="1" xr2:uid="{5D18506F-4356-4788-9DC5-6D9F3B187B49}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{5D18506F-4356-4788-9DC5-6D9F3B187B49}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefs Template" sheetId="1" r:id="rId1"/>
@@ -1357,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56457AC2-4CCE-48AB-B957-6565BDA2DBE4}">
   <dimension ref="B2:J59"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1413,11 +1413,11 @@
       </c>
       <c r="H3" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1, 6), "Overnight", "Biking","Spelunking", "Watersports", "Surfing", "Sea Kayaking")</f>
-        <v>Watersports</v>
+        <v>Spelunking</v>
       </c>
       <c r="J3">
         <f ca="1">CHOOSE(RANDBETWEEN(1, 2), 2, 4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2553,8 +2553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445B6131-D158-4A66-8748-C0EBB6C75469}">
   <dimension ref="B3:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3096,6 +3096,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1eec4c4c-619d-4796-91a6-89c807311e80">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7ad6aa05-2b5c-4683-81b2-fe78918efd15" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EE21F9AAB78248498383FA53BEB374BA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="163ad25bbb507060862b3df4f72e9a12">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1eec4c4c-619d-4796-91a6-89c807311e80" xmlns:ns3="7ad6aa05-2b5c-4683-81b2-fe78918efd15" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="15c63a09851a93e181ca14e181e763c2" ns2:_="" ns3:_="">
     <xsd:import namespace="1eec4c4c-619d-4796-91a6-89c807311e80"/>
@@ -3324,27 +3344,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1eec4c4c-619d-4796-91a6-89c807311e80">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7ad6aa05-2b5c-4683-81b2-fe78918efd15" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCA4C34A-1173-435D-BDBC-FEA8FF547DE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75092B96-EF1C-4949-8CF0-BA6FA8CE960D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1eec4c4c-619d-4796-91a6-89c807311e80"/>
+    <ds:schemaRef ds:uri="7ad6aa05-2b5c-4683-81b2-fe78918efd15"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3AB0F574-80C6-4CA8-AC85-8EBD37A88E5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3361,23 +3380,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75092B96-EF1C-4949-8CF0-BA6FA8CE960D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1eec4c4c-619d-4796-91a6-89c807311e80"/>
-    <ds:schemaRef ds:uri="7ad6aa05-2b5c-4683-81b2-fe78918efd15"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCA4C34A-1173-435D-BDBC-FEA8FF547DE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>